<commit_message>
zoom color ok, get last time data ok
</commit_message>
<xml_diff>
--- a/QuanLyKS/bin/Debug/CurrentCustomer.xlsx
+++ b/QuanLyKS/bin/Debug/CurrentCustomer.xlsx
@@ -372,7 +372,7 @@
   <dimension ref="A1:D26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B16" sqref="B16"/>
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -406,7 +406,7 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B3">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="D3">
         <v>0</v>
@@ -446,7 +446,7 @@
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B16">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="D16">
         <v>0</v>

</xml_diff>

<commit_message>
fill data vao gridview - chua chuyen doi dc giua cac phong
</commit_message>
<xml_diff>
--- a/QuanLyKS/bin/Debug/CurrentCustomer.xlsx
+++ b/QuanLyKS/bin/Debug/CurrentCustomer.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="24">
   <si>
     <t>Nguyễn Ngọc Anh</t>
   </si>
@@ -49,6 +49,48 @@
   </si>
   <si>
     <t>P102</t>
+  </si>
+  <si>
+    <t>P103</t>
+  </si>
+  <si>
+    <t>P104</t>
+  </si>
+  <si>
+    <t>P105</t>
+  </si>
+  <si>
+    <t>P106</t>
+  </si>
+  <si>
+    <t>P107</t>
+  </si>
+  <si>
+    <t>P108</t>
+  </si>
+  <si>
+    <t>P201</t>
+  </si>
+  <si>
+    <t>P202</t>
+  </si>
+  <si>
+    <t>P203</t>
+  </si>
+  <si>
+    <t>P204</t>
+  </si>
+  <si>
+    <t>P205</t>
+  </si>
+  <si>
+    <t>P206</t>
+  </si>
+  <si>
+    <t>P207</t>
+  </si>
+  <si>
+    <t>Fanta</t>
   </si>
 </sst>
 </file>
@@ -369,10 +411,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D26"/>
+  <dimension ref="A1:D195"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="C17" sqref="C17"/>
+    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
+      <selection activeCell="C45" sqref="C45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -446,7 +488,7 @@
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B16">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="D16">
         <v>0</v>
@@ -462,6 +504,546 @@
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="D26">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>7</v>
+      </c>
+      <c r="B27" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>6</v>
+      </c>
+      <c r="B28" t="s">
+        <v>10</v>
+      </c>
+      <c r="C28" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B29">
+        <v>5</v>
+      </c>
+      <c r="D29">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>3</v>
+      </c>
+      <c r="B30">
+        <v>400000</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D39">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
+        <v>7</v>
+      </c>
+      <c r="B40" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
+        <v>6</v>
+      </c>
+      <c r="B41" t="s">
+        <v>11</v>
+      </c>
+      <c r="C41" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B42">
+        <v>5</v>
+      </c>
+      <c r="D42">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A43" t="s">
+        <v>3</v>
+      </c>
+      <c r="B43">
+        <v>300000</v>
+      </c>
+      <c r="C43">
+        <v>3</v>
+      </c>
+      <c r="D43">
+        <v>900000</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A44" t="s">
+        <v>23</v>
+      </c>
+      <c r="B44">
+        <v>15000</v>
+      </c>
+      <c r="C44">
+        <v>10</v>
+      </c>
+      <c r="D44">
+        <v>45000</v>
+      </c>
+    </row>
+    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D52">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A53" t="s">
+        <v>7</v>
+      </c>
+      <c r="B53" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A54" t="s">
+        <v>6</v>
+      </c>
+      <c r="B54" t="s">
+        <v>12</v>
+      </c>
+      <c r="C54" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B55">
+        <v>8</v>
+      </c>
+      <c r="D55">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A56" t="s">
+        <v>3</v>
+      </c>
+      <c r="B56">
+        <v>400000</v>
+      </c>
+    </row>
+    <row r="65" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D65">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="66" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A66" t="s">
+        <v>7</v>
+      </c>
+      <c r="B66" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="67" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A67" t="s">
+        <v>6</v>
+      </c>
+      <c r="B67" t="s">
+        <v>13</v>
+      </c>
+      <c r="C67" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="68" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B68">
+        <v>8</v>
+      </c>
+      <c r="D68">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="69" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A69" t="s">
+        <v>3</v>
+      </c>
+      <c r="B69">
+        <v>400000</v>
+      </c>
+    </row>
+    <row r="78" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D78">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="79" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A79" t="s">
+        <v>7</v>
+      </c>
+      <c r="B79" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="80" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A80" t="s">
+        <v>6</v>
+      </c>
+      <c r="B80" t="s">
+        <v>14</v>
+      </c>
+      <c r="C80" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="81" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B81">
+        <v>8</v>
+      </c>
+      <c r="D81">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="82" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A82" t="s">
+        <v>3</v>
+      </c>
+      <c r="B82">
+        <v>400000</v>
+      </c>
+    </row>
+    <row r="91" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D91">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="92" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A92" t="s">
+        <v>7</v>
+      </c>
+      <c r="B92" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="93" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A93" t="s">
+        <v>6</v>
+      </c>
+      <c r="B93" t="s">
+        <v>15</v>
+      </c>
+      <c r="C93" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="94" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B94">
+        <v>8</v>
+      </c>
+      <c r="D94">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="95" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A95" t="s">
+        <v>3</v>
+      </c>
+      <c r="B95">
+        <v>400000</v>
+      </c>
+    </row>
+    <row r="104" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D104">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="105" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A105" t="s">
+        <v>7</v>
+      </c>
+      <c r="B105" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="106" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A106" t="s">
+        <v>6</v>
+      </c>
+      <c r="B106" t="s">
+        <v>16</v>
+      </c>
+      <c r="C106" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="107" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B107">
+        <v>8</v>
+      </c>
+      <c r="D107">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="108" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A108" t="s">
+        <v>3</v>
+      </c>
+      <c r="B108">
+        <v>400000</v>
+      </c>
+    </row>
+    <row r="117" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D117">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="118" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A118" t="s">
+        <v>7</v>
+      </c>
+      <c r="B118" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="119" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A119" t="s">
+        <v>6</v>
+      </c>
+      <c r="B119" t="s">
+        <v>17</v>
+      </c>
+      <c r="C119" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="120" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B120">
+        <v>8</v>
+      </c>
+      <c r="D120">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="121" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A121" t="s">
+        <v>3</v>
+      </c>
+      <c r="B121">
+        <v>400000</v>
+      </c>
+    </row>
+    <row r="130" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D130">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="131" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A131" t="s">
+        <v>7</v>
+      </c>
+      <c r="B131" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="132" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A132" t="s">
+        <v>6</v>
+      </c>
+      <c r="B132" t="s">
+        <v>18</v>
+      </c>
+      <c r="C132" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="133" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B133">
+        <v>8</v>
+      </c>
+      <c r="D133">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="134" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A134" t="s">
+        <v>3</v>
+      </c>
+      <c r="B134">
+        <v>400000</v>
+      </c>
+    </row>
+    <row r="143" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D143">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="144" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A144" t="s">
+        <v>7</v>
+      </c>
+      <c r="B144" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="145" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A145" t="s">
+        <v>6</v>
+      </c>
+      <c r="B145" t="s">
+        <v>19</v>
+      </c>
+      <c r="C145" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="146" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B146">
+        <v>8</v>
+      </c>
+      <c r="D146">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="147" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A147" t="s">
+        <v>3</v>
+      </c>
+      <c r="B147">
+        <v>400000</v>
+      </c>
+    </row>
+    <row r="156" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D156">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="157" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A157" t="s">
+        <v>7</v>
+      </c>
+      <c r="B157" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="158" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A158" t="s">
+        <v>6</v>
+      </c>
+      <c r="B158" t="s">
+        <v>20</v>
+      </c>
+      <c r="C158" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="159" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B159">
+        <v>8</v>
+      </c>
+      <c r="D159">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="160" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A160" t="s">
+        <v>3</v>
+      </c>
+      <c r="B160">
+        <v>400000</v>
+      </c>
+    </row>
+    <row r="169" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D169">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="170" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A170" t="s">
+        <v>7</v>
+      </c>
+      <c r="B170" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="171" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A171" t="s">
+        <v>6</v>
+      </c>
+      <c r="B171" t="s">
+        <v>21</v>
+      </c>
+      <c r="C171" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="172" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B172">
+        <v>8</v>
+      </c>
+      <c r="D172">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="173" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A173" t="s">
+        <v>3</v>
+      </c>
+      <c r="B173">
+        <v>400000</v>
+      </c>
+    </row>
+    <row r="182" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D182">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="183" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A183" t="s">
+        <v>7</v>
+      </c>
+      <c r="B183" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="184" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A184" t="s">
+        <v>6</v>
+      </c>
+      <c r="B184" t="s">
+        <v>22</v>
+      </c>
+      <c r="C184" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="185" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B185">
+        <v>8</v>
+      </c>
+      <c r="D185">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="186" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A186" t="s">
+        <v>3</v>
+      </c>
+      <c r="B186">
+        <v>400000</v>
+      </c>
+    </row>
+    <row r="195" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D195">
         <v>0</v>
       </c>
     </row>

</xml_diff>